<commit_message>
Minor updates to parser output
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_programs\SCHOOL\MSD\GIT\core\ts_core\excel_parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF34E838-12B3-4FB5-81F8-E1DE7BEAA6E8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173C9CEA-7C28-4515-8325-C0560780B44B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>SUMO Attribute</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Unused</t>
   </si>
   <si>
-    <t>numLanes</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
@@ -276,10 +273,13 @@
     <t>outbound_node</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
     <t>Outbound Intersection ID</t>
+  </si>
+  <si>
+    <t>inbound_lanes</t>
+  </si>
+  <si>
+    <t>This branches ID for output</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -739,23 +739,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF1932"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1309,10 +1292,10 @@
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -1324,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>46</v>
@@ -1335,7 +1318,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
@@ -1344,7 +1327,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="12">
         <v>1</v>
@@ -1369,22 +1352,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsBlanks" dxfId="33" priority="6">
+    <cfRule type="containsBlanks" dxfId="31" priority="6">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="5">
       <formula>LEN(TRIM(F4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsBlanks" dxfId="31" priority="2">
+    <cfRule type="containsBlanks" dxfId="29" priority="2">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="1">
       <formula>LEN(TRIM(F3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1495,7 +1478,7 @@
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsBlanks" dxfId="29" priority="1">
+    <cfRule type="containsBlanks" dxfId="27" priority="1">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1513,7 +1496,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D23"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1526,10 +1509,11 @@
     <col min="6" max="9" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="12" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1569,7 +1553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="14" t="s">
         <v>24</v>
       </c>
@@ -1583,9 +1567,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
@@ -1613,10 +1597,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
@@ -1644,14 +1628,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>16</v>
@@ -1670,9 +1654,9 @@
       </c>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1698,14 +1682,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>16</v>
@@ -1724,9 +1708,9 @@
       </c>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1752,9 +1736,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>37</v>
@@ -1786,14 +1770,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8">
@@ -1812,31 +1796,34 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2</v>
+      </c>
+      <c r="H13" s="8">
+        <v>3</v>
+      </c>
+      <c r="I13" s="8">
+        <v>4</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="L13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1848,8 +1835,8 @@
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>51</v>
       </c>
@@ -1883,7 +1870,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>50</v>
@@ -1913,12 +1900,12 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
@@ -1936,7 +1923,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1967,12 +1954,12 @@
     </row>
     <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="30" t="s">
@@ -2010,62 +1997,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F4:I4 F17:I17 F19:I19">
-    <cfRule type="containsBlanks" dxfId="28" priority="34">
+    <cfRule type="containsBlanks" dxfId="26" priority="34">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:I4 F17:I17 F19:I19">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="33">
       <formula>LEN(TRIM(F4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6">
-    <cfRule type="containsBlanks" dxfId="26" priority="28">
+    <cfRule type="containsBlanks" dxfId="24" priority="28">
       <formula>LEN(TRIM(F6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="27">
       <formula>LEN(TRIM(F6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:I8">
-    <cfRule type="containsBlanks" dxfId="24" priority="8">
+    <cfRule type="containsBlanks" dxfId="22" priority="8">
       <formula>LEN(TRIM(F8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:I8">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="7">
       <formula>LEN(TRIM(F8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:I16">
-    <cfRule type="containsBlanks" dxfId="22" priority="16">
+    <cfRule type="containsBlanks" dxfId="20" priority="16">
       <formula>LEN(TRIM(F16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:I16">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="15">
       <formula>LEN(TRIM(F16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:I20">
-    <cfRule type="containsBlanks" dxfId="20" priority="12">
+    <cfRule type="containsBlanks" dxfId="18" priority="12">
       <formula>LEN(TRIM(F20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:I20">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="11">
       <formula>LEN(TRIM(F20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:I10">
-    <cfRule type="containsBlanks" dxfId="18" priority="10">
+    <cfRule type="containsBlanks" dxfId="16" priority="10">
       <formula>LEN(TRIM(F10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:I10">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="9">
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Parser updates to include Stats file
Stats file is now generated in the parser. workHours and busLines are
not complete.
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="175">
   <si>
     <t>SUMO Attribute</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Proportion of the outgoing vehicles, leaving the city through this gate</t>
   </si>
   <si>
-    <t>School</t>
-  </si>
-  <si>
     <t>capacity</t>
   </si>
   <si>
@@ -549,6 +546,12 @@
   </si>
   <si>
     <t>Angle</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Schools</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2032,27 +2035,27 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F14" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F14" s="30" t="s">
+      <c r="G14" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="H14" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="I14" s="30" t="s">
         <v>170</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="J14" s="9"/>
     </row>
@@ -2360,9 +2363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2902,7 +2905,7 @@
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -2926,7 +2929,7 @@
         <v>123</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>123</v>
@@ -3446,7 +3449,7 @@
       <c r="A60" s="18"/>
       <c r="B60" s="18"/>
       <c r="C60" s="36" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
@@ -3534,7 +3537,7 @@
         <v>136</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>140</v>
@@ -3558,10 +3561,10 @@
         <v>108</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E64" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F64" s="2">
         <v>12</v>
@@ -3582,7 +3585,7 @@
         <v>109</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E65" s="32" t="s">
         <v>115</v>
@@ -3603,10 +3606,10 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E66" s="32"/>
       <c r="F66" s="2">
@@ -3625,10 +3628,10 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D67" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E67" s="32"/>
       <c r="F67" s="2">
@@ -3647,10 +3650,10 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E68" s="32"/>
       <c r="F68" s="2">
@@ -3714,7 +3717,7 @@
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
       <c r="C73" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
@@ -3802,7 +3805,7 @@
         <v>136</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F76" s="2">
         <v>456</v>
@@ -3817,7 +3820,7 @@
         <v>56</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E77" s="32"/>
       <c r="F77" s="2">
@@ -3881,7 +3884,7 @@
       <c r="A82" s="18"/>
       <c r="B82" s="18"/>
       <c r="C82" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
@@ -3899,7 +3902,7 @@
         <v>56</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E83" s="32"/>
       <c r="F83" s="2">
@@ -3912,10 +3915,10 @@
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E84" s="32"/>
       <c r="F84" s="2">
@@ -3925,10 +3928,10 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D85" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E85" s="32"/>
       <c r="F85" s="2">
@@ -3938,7 +3941,7 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="2">
@@ -3948,7 +3951,7 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E87" s="32"/>
       <c r="F87" s="2">
@@ -3958,7 +3961,7 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E88" s="32"/>
       <c r="F88" s="2">
@@ -4009,7 +4012,7 @@
       <c r="M90" s="11"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:J34">
       <formula1>"Opening, Closing"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Removed unnecessary print statements
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="1" r:id="rId1"/>
@@ -2365,7 +2365,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Fixed Excel template to match example intersection
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="176">
   <si>
     <t>SUMO Attribute</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>Schools</t>
+  </si>
+  <si>
+    <t>proportion</t>
   </si>
 </sst>
 </file>
@@ -2364,8 +2367,8 @@
   <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2683,7 +2686,7 @@
         <v>102</v>
       </c>
       <c r="F17" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -2737,7 +2740,7 @@
         <v>104</v>
       </c>
       <c r="F20" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -2755,7 +2758,7 @@
         <v>106</v>
       </c>
       <c r="F21" s="9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2962,7 +2965,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="2" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="D36" s="32" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
excel sheet and parser updates:
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_programs\SCHOOL\MSD\GIT\core\ts_core\excel_parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eilifm/github/eilifm/trafficsense/core/ts_core/excel_parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28420" windowHeight="13740" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Branch Settings" sheetId="7" r:id="rId3"/>
     <sheet name="Advanced Customization" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="177">
   <si>
     <t>SUMO Attribute</t>
   </si>
@@ -552,15 +552,28 @@
   </si>
   <si>
     <t>Schools</t>
+  </si>
+  <si>
+    <t>sensor_start</t>
+  </si>
+  <si>
+    <t>sensor_end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -884,52 +897,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1448,7 +1462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1456,20 +1470,20 @@
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+    <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" hidden="1" thickBot="1">
+    <row r="2" spans="1:7" ht="17" hidden="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1500,7 +1514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1">
+    <row r="3" spans="1:7" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -1582,16 +1596,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Years, Months, Days, Hours"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Extremely low, low, Moderate, Medium, Heavy, Rush-Hour"</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1599,27 +1613,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1">
+    <row r="1" spans="1:8" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1690,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" thickBot="1">
+    <row r="5" spans="1:8" ht="17" thickBot="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1693,7 +1707,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Cross, T, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1702,28 +1716,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+    <row r="1" spans="1:12" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1763,7 +1777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1">
+    <row r="3" spans="1:12" ht="17" thickBot="1">
       <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1777,7 +1791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" thickBot="1">
+    <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="A4" s="15" t="s">
         <v>55</v>
       </c>
@@ -1807,7 +1821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16.5" thickBot="1"/>
+    <row r="5" spans="1:12" ht="17" thickBot="1"/>
     <row r="6" spans="1:12">
       <c r="A6" s="18" t="s">
         <v>50</v>
@@ -2059,7 +2073,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickBot="1">
+    <row r="15" spans="1:12" ht="17" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2071,7 +2085,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickBot="1"/>
+    <row r="16" spans="1:12" ht="17" thickBot="1"/>
     <row r="17" spans="1:12">
       <c r="A17" s="4" t="s">
         <v>37</v>
@@ -2188,40 +2202,76 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
+        <v>50</v>
+      </c>
+      <c r="G21" s="8">
+        <v>50</v>
+      </c>
+      <c r="H21" s="8">
+        <v>50</v>
+      </c>
+      <c r="I21" s="8">
+        <v>50</v>
+      </c>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8">
+        <v>100</v>
+      </c>
+      <c r="G22" s="8">
+        <v>100</v>
+      </c>
+      <c r="H22" s="8">
+        <v>100</v>
+      </c>
+      <c r="I22" s="8">
+        <v>100</v>
+      </c>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" ht="17" thickBot="1">
+      <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="27" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G23" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H23" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I23" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="F25" s="8"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="29" spans="1:12">
       <c r="G29" s="8"/>
@@ -2231,13 +2281,21 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
+    <row r="31" spans="1:12">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I20">
+  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I22">
     <cfRule type="containsBlanks" dxfId="17" priority="36">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I20">
+  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I22">
     <cfRule type="notContainsBlanks" dxfId="16" priority="35">
       <formula>LEN(TRIM(F4))&gt;0</formula>
     </cfRule>
@@ -2272,14 +2330,14 @@
       <formula>LEN(TRIM(F17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I21">
+  <conditionalFormatting sqref="F23:I23">
     <cfRule type="containsBlanks" dxfId="9" priority="14">
-      <formula>LEN(TRIM(F21))=0</formula>
+      <formula>LEN(TRIM(F23))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I21">
+  <conditionalFormatting sqref="F23:I23">
     <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(F21))&gt;0</formula>
+      <formula>LEN(TRIM(F23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:I10">
@@ -2323,34 +2381,34 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:I4 F15:I15 F20:I20 F17:I18">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:I4 F15:I15 F20:I22 F17:I18" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Miles per Hour, Kilometers per Hour"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Feet, Miles, Meters, Kilometers"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21:I21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:I23" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Priority"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:I6 F10:I10 F8:I8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:I6 F10:I10 F8:I8" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:I21">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:I23" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Priority"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Priority, sdfg"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:I14">
+    <dataValidation type="list" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:I14" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"N, NE, E, SE, S, SW, W, NW"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2360,33 +2418,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="13" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="48.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1">
+    <row r="1" spans="1:18" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2442,7 +2500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="16.5" thickBot="1">
+    <row r="2" spans="1:18" ht="17" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2644,7 +2702,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:18" ht="16.5" thickBot="1">
+    <row r="13" spans="1:18" ht="17" thickBot="1">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -2654,7 +2712,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="15" spans="1:18" ht="16.5" thickBot="1">
+    <row r="15" spans="1:18" ht="17" thickBot="1">
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
@@ -2760,7 +2818,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1">
+    <row r="22" spans="1:10" ht="17" thickBot="1">
       <c r="A22" s="25"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -2774,7 +2832,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="16.5" thickBot="1">
+    <row r="24" spans="1:10" ht="17" thickBot="1">
       <c r="D24" s="2" t="s">
         <v>114</v>
       </c>
@@ -2886,7 +2944,7 @@
       </c>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" ht="16.5" thickBot="1">
+    <row r="30" spans="1:10" ht="17" thickBot="1">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -2898,7 +2956,7 @@
       <c r="I30" s="25"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="32" spans="1:10" ht="16.5" thickBot="1">
+    <row r="32" spans="1:10" ht="17" thickBot="1">
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="1:13">
@@ -2997,7 +3055,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16.5" thickBot="1">
+    <row r="38" spans="1:13" ht="17" thickBot="1">
       <c r="A38" s="25"/>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -3009,7 +3067,7 @@
       <c r="I38" s="25"/>
       <c r="J38" s="11"/>
     </row>
-    <row r="40" spans="1:13" ht="16.5" thickBot="1"/>
+    <row r="40" spans="1:13" ht="17" thickBot="1"/>
     <row r="41" spans="1:13">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
@@ -3194,7 +3252,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="16.5" thickBot="1">
+    <row r="47" spans="1:13" ht="17" thickBot="1">
       <c r="A47" s="25"/>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
@@ -3209,7 +3267,7 @@
       <c r="L47" s="25"/>
       <c r="M47" s="11"/>
     </row>
-    <row r="49" spans="1:13" ht="16.5" thickBot="1"/>
+    <row r="49" spans="1:13" ht="17" thickBot="1"/>
     <row r="50" spans="1:13">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
@@ -3429,7 +3487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="16.5" thickBot="1">
+    <row r="57" spans="1:13" ht="17" thickBot="1">
       <c r="A57" s="25"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
@@ -3444,7 +3502,7 @@
       <c r="L57" s="25"/>
       <c r="M57" s="11"/>
     </row>
-    <row r="59" spans="1:13" ht="16.5" thickBot="1"/>
+    <row r="59" spans="1:13" ht="17" thickBot="1"/>
     <row r="60" spans="1:13">
       <c r="A60" s="18"/>
       <c r="B60" s="18"/>
@@ -3697,7 +3755,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="16.5" thickBot="1">
+    <row r="70" spans="1:13" ht="17" thickBot="1">
       <c r="A70" s="25"/>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
@@ -3712,7 +3770,7 @@
       <c r="L70" s="25"/>
       <c r="M70" s="11"/>
     </row>
-    <row r="72" spans="1:13" ht="16.5" thickBot="1"/>
+    <row r="72" spans="1:13" ht="17" thickBot="1"/>
     <row r="73" spans="1:13">
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
@@ -3858,7 +3916,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16.5" thickBot="1">
+    <row r="79" spans="1:13" ht="17" thickBot="1">
       <c r="A79" s="25"/>
       <c r="B79" s="25"/>
       <c r="C79" s="25"/>
@@ -3877,7 +3935,7 @@
       <c r="D80" s="32"/>
       <c r="E80" s="32"/>
     </row>
-    <row r="81" spans="1:13" ht="16.5" thickBot="1">
+    <row r="81" spans="1:13" ht="17" thickBot="1">
       <c r="D81" s="32"/>
     </row>
     <row r="82" spans="1:13">
@@ -3996,7 +4054,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="16.5" thickBot="1">
+    <row r="90" spans="1:13" ht="17" thickBot="1">
       <c r="A90" s="25"/>
       <c r="B90" s="25"/>
       <c r="C90" s="25"/>
@@ -4013,13 +4071,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:J34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:J34" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Opening, Closing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:M42 F51:M51 F61:M61 F74:M74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:M42 F51:M51 F61:M61 F74:M74" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"1, 2, 3, 4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:M43 F52:M52 F62:M62 F75:M75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:M43 F52:M52 F62:M62 F75:M75" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"Inbound, Outbound"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated docstrings - Some file management
Added the 4 examples shown during ImagineRIT. Foxed Docstrings to use
numpy format. Removed some unnecessary files introduced in the past.
</commit_message>
<xml_diff>
--- a/ts_core/excel_parser/Configuration_template.xlsx
+++ b/ts_core/excel_parser/Configuration_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_programs\SCHOOL\MSD\GIT\core\ts_core\excel_parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eilifm/github/eilifm/trafficsense/core/ts_core/excel_parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28420" windowHeight="13740" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Branch Settings" sheetId="7" r:id="rId3"/>
     <sheet name="Advanced Customization" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="177">
   <si>
     <t>SUMO Attribute</t>
   </si>
@@ -554,16 +554,26 @@
     <t>Schools</t>
   </si>
   <si>
-    <t>proportion</t>
+    <t>sensor_start</t>
+  </si>
+  <si>
+    <t>sensor_end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -595,13 +605,16 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000040"/>
-      <name val="Monotype"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF252525"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -887,50 +900,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1451,7 +1473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1459,20 +1481,20 @@
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+    <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" hidden="1" thickBot="1">
+    <row r="2" spans="1:7" ht="17" hidden="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1503,7 +1525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1">
+    <row r="3" spans="1:7" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -1585,16 +1607,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Years, Months, Days, Hours"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Extremely low, low, Moderate, Medium, Heavy, Rush-Hour"</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1602,27 +1624,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1">
+    <row r="1" spans="1:8" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1701,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" thickBot="1">
+    <row r="5" spans="1:8" ht="17" thickBot="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1696,7 +1718,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Cross, T, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1705,28 +1727,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+    <row r="1" spans="1:12" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1">
+    <row r="3" spans="1:12" ht="17" thickBot="1">
       <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1780,7 +1802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" thickBot="1">
+    <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="A4" s="15" t="s">
         <v>55</v>
       </c>
@@ -1810,7 +1832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16.5" thickBot="1"/>
+    <row r="5" spans="1:12" ht="17" thickBot="1"/>
     <row r="6" spans="1:12">
       <c r="A6" s="18" t="s">
         <v>50</v>
@@ -1825,16 +1847,16 @@
       <c r="E6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="26">
         <v>0</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="26">
         <v>0</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="26">
         <v>0</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="26">
         <v>0</v>
       </c>
       <c r="J6" s="19" t="s">
@@ -1853,16 +1875,16 @@
       <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="27">
         <v>1</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="27">
         <v>1</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="27">
         <v>1</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="27">
         <v>1</v>
       </c>
       <c r="J7" s="20"/>
@@ -1879,16 +1901,16 @@
       <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="28">
         <v>1</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="28">
         <v>1</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="28">
         <v>1</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="28">
         <v>1</v>
       </c>
       <c r="J8" s="20" t="s">
@@ -1907,16 +1929,16 @@
       <c r="E9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="27">
         <v>1</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="27">
         <v>1</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="27">
         <v>1</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="27">
         <v>1</v>
       </c>
       <c r="J9" s="20"/>
@@ -1933,16 +1955,16 @@
       <c r="E10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>0</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="28">
         <v>0</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>0</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="28">
         <v>0</v>
       </c>
       <c r="J10" s="9" t="s">
@@ -2048,21 +2070,21 @@
       <c r="E14" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="28" t="s">
         <v>170</v>
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickBot="1">
+    <row r="15" spans="1:12" ht="17" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2074,7 +2096,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickBot="1"/>
+    <row r="16" spans="1:12" ht="17" thickBot="1"/>
     <row r="17" spans="1:12">
       <c r="A17" s="4" t="s">
         <v>37</v>
@@ -2191,40 +2213,76 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
+        <v>50</v>
+      </c>
+      <c r="G21" s="8">
+        <v>50</v>
+      </c>
+      <c r="H21" s="8">
+        <v>50</v>
+      </c>
+      <c r="I21" s="8">
+        <v>50</v>
+      </c>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8">
+        <v>100</v>
+      </c>
+      <c r="G22" s="8">
+        <v>100</v>
+      </c>
+      <c r="H22" s="8">
+        <v>100</v>
+      </c>
+      <c r="I22" s="8">
+        <v>100</v>
+      </c>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" ht="17" thickBot="1">
+      <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="27" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G23" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H23" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I23" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="F25" s="8"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="29" spans="1:12">
       <c r="G29" s="8"/>
@@ -2234,13 +2292,21 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
+    <row r="31" spans="1:12">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I20">
+  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I22">
     <cfRule type="containsBlanks" dxfId="17" priority="36">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I20">
+  <conditionalFormatting sqref="F4:I4 F18:I18 F20:I22">
     <cfRule type="notContainsBlanks" dxfId="16" priority="35">
       <formula>LEN(TRIM(F4))&gt;0</formula>
     </cfRule>
@@ -2275,14 +2341,14 @@
       <formula>LEN(TRIM(F17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I21">
+  <conditionalFormatting sqref="F23:I23">
     <cfRule type="containsBlanks" dxfId="9" priority="14">
-      <formula>LEN(TRIM(F21))=0</formula>
+      <formula>LEN(TRIM(F23))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I21">
+  <conditionalFormatting sqref="F23:I23">
     <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(F21))&gt;0</formula>
+      <formula>LEN(TRIM(F23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:I10">
@@ -2326,34 +2392,34 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:I4 F15:I15 F20:I20 F17:I18">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:I4 F15:I15 F20:I22 F17:I18" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Miles per Hour, Kilometers per Hour"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Feet, Miles, Meters, Kilometers"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21:I21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:I23" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Priority"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:I6 F10:I10 F8:I8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:I6 F10:I10 F8:I8" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:I21">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:I23" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Priority"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Priority, sdfg"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:I9 F7:I7" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:I14">
+    <dataValidation type="list" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:I14" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"N, NE, E, SE, S, SW, W, NW"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2363,33 +2429,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="13" style="30" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1">
+    <row r="1" spans="1:18" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2445,1584 +2511,1584 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="16.5" thickBot="1">
+    <row r="2" spans="1:18" ht="17" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="33"/>
+      <c r="E2" s="31"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="34"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="35">
         <v>1000</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="35">
         <v>500</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="35">
         <v>18</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="32" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="35">
         <v>65</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="35">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="35">
         <v>0.05</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="32" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="35">
         <v>350</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="35">
         <v>200</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="35">
         <v>50</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" ht="16.5" thickBot="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="15" spans="1:18" ht="16.5" thickBot="1">
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:18" ht="17" thickBot="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="15" spans="1:18" ht="17" thickBot="1">
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="34"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="35">
+        <v>0</v>
+      </c>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="35">
+        <v>360</v>
+      </c>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="35">
+        <v>0.15</v>
+      </c>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="35">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="35">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" ht="17" thickBot="1">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" ht="17" thickBot="1">
+      <c r="D24" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="J24" s="41"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="29">
+        <v>0</v>
+      </c>
+      <c r="G26" s="29">
+        <v>15</v>
+      </c>
+      <c r="H26" s="29">
+        <v>31</v>
+      </c>
+      <c r="I26" s="29">
+        <v>60</v>
+      </c>
+      <c r="J26" s="35"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="30">
+        <v>15</v>
+      </c>
+      <c r="G27" s="29">
+        <v>30</v>
+      </c>
+      <c r="H27" s="29">
+        <v>60</v>
+      </c>
+      <c r="I27" s="30">
+        <v>90</v>
+      </c>
+      <c r="J27" s="35"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="30">
+        <v>5000</v>
+      </c>
+      <c r="G28" s="29">
+        <v>10000</v>
+      </c>
+      <c r="H28" s="29">
+        <v>17450</v>
+      </c>
+      <c r="I28" s="30">
+        <v>9780</v>
+      </c>
+      <c r="J28" s="35"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="D29" s="37"/>
+      <c r="F29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="35"/>
+    </row>
+    <row r="30" spans="1:10" ht="17" thickBot="1">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="42"/>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickBot="1">
+      <c r="J32" s="41"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="30">
+        <v>600</v>
+      </c>
+      <c r="G35" s="29">
+        <v>43200</v>
+      </c>
+      <c r="H35" s="29"/>
+      <c r="J35" s="35"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="G36" s="29">
+        <v>0.2</v>
+      </c>
+      <c r="H36" s="29"/>
+      <c r="J36" s="35"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="D37" s="37"/>
+      <c r="F37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="17" thickBot="1">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="42"/>
+    </row>
+    <row r="40" spans="1:13" ht="17" thickBot="1"/>
+    <row r="41" spans="1:13">
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="34"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29">
+        <v>1</v>
+      </c>
+      <c r="G42" s="29">
+        <v>1</v>
+      </c>
+      <c r="H42" s="29">
+        <v>2</v>
+      </c>
+      <c r="I42" s="29">
+        <v>2</v>
+      </c>
+      <c r="J42" s="29">
+        <v>3</v>
+      </c>
+      <c r="K42" s="29">
+        <v>3</v>
+      </c>
+      <c r="L42" s="29">
+        <v>4</v>
+      </c>
+      <c r="M42" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="I43" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="J43" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="K43" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="L43" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M43" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="G44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="H44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="I44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="J44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="K44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="L44" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="M44" s="35">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" s="30">
+        <v>10</v>
+      </c>
+      <c r="G45" s="30">
+        <v>10</v>
+      </c>
+      <c r="H45" s="30">
+        <v>10</v>
+      </c>
+      <c r="I45" s="30">
+        <v>10</v>
+      </c>
+      <c r="J45" s="30">
+        <v>10</v>
+      </c>
+      <c r="K45" s="30">
+        <v>10</v>
+      </c>
+      <c r="L45" s="30">
+        <v>10</v>
+      </c>
+      <c r="M45" s="35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="D46" s="37"/>
+      <c r="F46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M46" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="17" thickBot="1">
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="42"/>
+    </row>
+    <row r="49" spans="1:13" ht="17" thickBot="1"/>
+    <row r="50" spans="1:13">
+      <c r="A50" s="33"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="34"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29">
+        <v>1</v>
+      </c>
+      <c r="G51" s="29">
+        <v>1</v>
+      </c>
+      <c r="H51" s="29">
+        <v>2</v>
+      </c>
+      <c r="I51" s="29">
+        <v>2</v>
+      </c>
+      <c r="J51" s="29">
+        <v>3</v>
+      </c>
+      <c r="K51" s="29">
+        <v>3</v>
+      </c>
+      <c r="L51" s="29">
+        <v>4</v>
+      </c>
+      <c r="M51" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="K52" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="L52" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M52" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" s="30">
+        <v>243</v>
+      </c>
+      <c r="G53" s="30">
+        <v>0</v>
+      </c>
+      <c r="H53" s="30">
+        <v>243</v>
+      </c>
+      <c r="I53" s="30">
+        <v>0</v>
+      </c>
+      <c r="J53" s="30">
+        <v>243</v>
+      </c>
+      <c r="K53" s="30">
+        <v>0</v>
+      </c>
+      <c r="L53" s="30">
+        <v>243</v>
+      </c>
+      <c r="M53" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="G54" s="30">
+        <v>1</v>
+      </c>
+      <c r="H54" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="I54" s="30">
+        <v>1</v>
+      </c>
+      <c r="J54" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="K54" s="30">
+        <v>1</v>
+      </c>
+      <c r="L54" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="M54" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G55" s="30">
         <v>0.5</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="9">
-        <v>360</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="9">
-        <v>120</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" ht="16.5" thickBot="1">
-      <c r="D24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="8" t="s">
+      <c r="H55" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I55" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="J55" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K55" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M55" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="D56" s="37"/>
+      <c r="F56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L56" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M56" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" thickBot="1">
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
+      <c r="M57" s="42"/>
+    </row>
+    <row r="59" spans="1:13" ht="17" thickBot="1"/>
+    <row r="60" spans="1:13">
+      <c r="A60" s="33"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="34"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29">
+        <v>1</v>
+      </c>
+      <c r="G61" s="29">
+        <v>2</v>
+      </c>
+      <c r="H61" s="29">
+        <v>3</v>
+      </c>
+      <c r="I61" s="29">
+        <v>4</v>
+      </c>
+      <c r="J61" s="29">
+        <v>3</v>
+      </c>
+      <c r="K61" s="29">
+        <v>3</v>
+      </c>
+      <c r="L61" s="29">
+        <v>4</v>
+      </c>
+      <c r="M61" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G62" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I62" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="J62" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="K62" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="L62" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M62" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F63" s="30">
+        <v>23</v>
+      </c>
+      <c r="G63" s="30">
+        <v>23</v>
+      </c>
+      <c r="H63" s="30">
+        <v>23</v>
+      </c>
+      <c r="I63" s="30">
+        <v>23</v>
+      </c>
+      <c r="M63" s="35"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8">
-        <v>15</v>
-      </c>
-      <c r="H26" s="8">
-        <v>31</v>
-      </c>
-      <c r="I26" s="8">
-        <v>60</v>
-      </c>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="2" t="s">
+      <c r="D64" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="E64" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="F64" s="30">
+        <v>12</v>
+      </c>
+      <c r="G64" s="30">
+        <v>12</v>
+      </c>
+      <c r="H64" s="30">
+        <v>12</v>
+      </c>
+      <c r="I64" s="30">
+        <v>12</v>
+      </c>
+      <c r="M64" s="35"/>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D65" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="F27" s="2">
-        <v>15</v>
-      </c>
-      <c r="G27" s="8">
-        <v>30</v>
-      </c>
-      <c r="H27" s="8">
-        <v>60</v>
-      </c>
-      <c r="I27" s="2">
-        <v>90</v>
-      </c>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="2">
-        <v>5000</v>
-      </c>
-      <c r="G28" s="8">
+      <c r="F65" s="30">
+        <v>18</v>
+      </c>
+      <c r="G65" s="30">
+        <v>18</v>
+      </c>
+      <c r="H65" s="30">
+        <v>18</v>
+      </c>
+      <c r="I65" s="30">
+        <v>18</v>
+      </c>
+      <c r="M65" s="35"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="37"/>
+      <c r="F66" s="30">
+        <v>400</v>
+      </c>
+      <c r="G66" s="30">
+        <v>400</v>
+      </c>
+      <c r="H66" s="30">
+        <v>400</v>
+      </c>
+      <c r="I66" s="30">
+        <v>400</v>
+      </c>
+      <c r="M66" s="35"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E67" s="37"/>
+      <c r="F67" s="30">
+        <v>32400</v>
+      </c>
+      <c r="G67" s="30">
+        <v>32400</v>
+      </c>
+      <c r="H67" s="30">
+        <v>32400</v>
+      </c>
+      <c r="I67" s="30">
+        <v>32400</v>
+      </c>
+      <c r="M67" s="35"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E68" s="37"/>
+      <c r="F68" s="30">
+        <v>64800</v>
+      </c>
+      <c r="G68" s="30">
+        <v>64800</v>
+      </c>
+      <c r="H68" s="30">
+        <v>64800</v>
+      </c>
+      <c r="I68" s="30">
+        <v>64800</v>
+      </c>
+      <c r="M68" s="35"/>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="D69" s="37"/>
+      <c r="F69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L69" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M69" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="17" thickBot="1">
+      <c r="A70" s="38"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="38"/>
+      <c r="L70" s="38"/>
+      <c r="M70" s="42"/>
+    </row>
+    <row r="72" spans="1:13" ht="17" thickBot="1"/>
+    <row r="73" spans="1:13">
+      <c r="A73" s="33"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="33"/>
+      <c r="M73" s="34"/>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29">
+        <v>2</v>
+      </c>
+      <c r="G74" s="29">
+        <v>4</v>
+      </c>
+      <c r="H74" s="29">
+        <v>3</v>
+      </c>
+      <c r="I74" s="29">
+        <v>4</v>
+      </c>
+      <c r="J74" s="29">
+        <v>3</v>
+      </c>
+      <c r="K74" s="29">
+        <v>3</v>
+      </c>
+      <c r="L74" s="29">
+        <v>4</v>
+      </c>
+      <c r="M74" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G75" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="J75" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="K75" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="L75" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M75" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F76" s="30">
+        <v>456</v>
+      </c>
+      <c r="G76" s="30">
+        <v>324</v>
+      </c>
+      <c r="M76" s="35"/>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" s="37"/>
+      <c r="F77" s="30">
+        <v>1</v>
+      </c>
+      <c r="G77" s="30">
+        <v>2</v>
+      </c>
+      <c r="M77" s="35"/>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="E78" s="37"/>
+      <c r="F78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L78" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M78" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="17" thickBot="1">
+      <c r="A79" s="38"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
+      <c r="L79" s="38"/>
+      <c r="M79" s="42"/>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+    </row>
+    <row r="81" spans="1:13" ht="17" thickBot="1">
+      <c r="D81" s="37"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="33"/>
+      <c r="J82" s="33"/>
+      <c r="K82" s="33"/>
+      <c r="L82" s="33"/>
+      <c r="M82" s="34"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E83" s="37"/>
+      <c r="F83" s="30">
+        <v>1</v>
+      </c>
+      <c r="G83" s="30">
+        <v>2</v>
+      </c>
+      <c r="M83" s="35"/>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D84" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E84" s="37"/>
+      <c r="F84" s="30">
+        <v>3000</v>
+      </c>
+      <c r="M84" s="35"/>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E85" s="37"/>
+      <c r="F85" s="30">
+        <v>1</v>
+      </c>
+      <c r="M85" s="35"/>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E86" s="37"/>
+      <c r="F86" s="30">
         <v>10000</v>
       </c>
-      <c r="H28" s="8">
-        <v>17450</v>
-      </c>
-      <c r="I28" s="2">
-        <v>9780</v>
-      </c>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="D29" s="32"/>
-      <c r="F29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="32" spans="1:10" ht="16.5" thickBot="1">
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="34"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="2">
-        <v>600</v>
-      </c>
-      <c r="G35" s="8">
-        <v>43200</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G36" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="H36" s="8"/>
-      <c r="J36" s="9"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="D37" s="32"/>
-      <c r="F37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="40" spans="1:13" ht="16.5" thickBot="1"/>
-    <row r="41" spans="1:13">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="34"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8">
-        <v>1</v>
-      </c>
-      <c r="G42" s="8">
-        <v>1</v>
-      </c>
-      <c r="H42" s="8">
-        <v>2</v>
-      </c>
-      <c r="I42" s="8">
-        <v>2</v>
-      </c>
-      <c r="J42" s="8">
-        <v>3</v>
-      </c>
-      <c r="K42" s="8">
-        <v>3</v>
-      </c>
-      <c r="L42" s="8">
-        <v>4</v>
-      </c>
-      <c r="M42" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M43" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="G44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="H44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="I44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="J44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="K44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="L44" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="M44" s="9">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D45" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F45" s="2">
-        <v>10</v>
-      </c>
-      <c r="G45" s="2">
-        <v>10</v>
-      </c>
-      <c r="H45" s="2">
-        <v>10</v>
-      </c>
-      <c r="I45" s="2">
-        <v>10</v>
-      </c>
-      <c r="J45" s="2">
-        <v>10</v>
-      </c>
-      <c r="K45" s="2">
-        <v>10</v>
-      </c>
-      <c r="L45" s="2">
-        <v>10</v>
-      </c>
-      <c r="M45" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="D46" s="32"/>
-      <c r="F46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="11"/>
-    </row>
-    <row r="49" spans="1:13" ht="16.5" thickBot="1"/>
-    <row r="50" spans="1:13">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="34"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8">
-        <v>1</v>
-      </c>
-      <c r="G51" s="8">
-        <v>1</v>
-      </c>
-      <c r="H51" s="8">
-        <v>2</v>
-      </c>
-      <c r="I51" s="8">
-        <v>2</v>
-      </c>
-      <c r="J51" s="8">
-        <v>3</v>
-      </c>
-      <c r="K51" s="8">
-        <v>3</v>
-      </c>
-      <c r="L51" s="8">
-        <v>4</v>
-      </c>
-      <c r="M51" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K52" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M52" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D53" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F53" s="2">
-        <v>243</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
-        <v>243</v>
-      </c>
-      <c r="I53" s="2">
-        <v>0</v>
-      </c>
-      <c r="J53" s="2">
-        <v>243</v>
-      </c>
-      <c r="K53" s="2">
-        <v>0</v>
-      </c>
-      <c r="L53" s="2">
-        <v>243</v>
-      </c>
-      <c r="M53" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="E54" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="F54" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G54" s="2">
-        <v>1</v>
-      </c>
-      <c r="H54" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="I54" s="2">
-        <v>1</v>
-      </c>
-      <c r="J54" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="K54" s="2">
-        <v>1</v>
-      </c>
-      <c r="L54" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="M54" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E55" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H55" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I55" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J55" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K55" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L55" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M55" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="D56" s="32"/>
-      <c r="F56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M56" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="11"/>
-    </row>
-    <row r="59" spans="1:13" ht="16.5" thickBot="1"/>
-    <row r="60" spans="1:13">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="18"/>
-      <c r="M60" s="34"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8">
-        <v>1</v>
-      </c>
-      <c r="G61" s="8">
-        <v>2</v>
-      </c>
-      <c r="H61" s="8">
-        <v>3</v>
-      </c>
-      <c r="I61" s="8">
-        <v>4</v>
-      </c>
-      <c r="J61" s="8">
-        <v>3</v>
-      </c>
-      <c r="K61" s="8">
-        <v>3</v>
-      </c>
-      <c r="L61" s="8">
-        <v>4</v>
-      </c>
-      <c r="M61" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K62" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="L62" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M62" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F63" s="2">
-        <v>23</v>
-      </c>
-      <c r="G63" s="2">
-        <v>23</v>
-      </c>
-      <c r="H63" s="2">
-        <v>23</v>
-      </c>
-      <c r="I63" s="2">
-        <v>23</v>
-      </c>
-      <c r="M63" s="9"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D64" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="F64" s="2">
-        <v>12</v>
-      </c>
-      <c r="G64" s="2">
-        <v>12</v>
-      </c>
-      <c r="H64" s="2">
-        <v>12</v>
-      </c>
-      <c r="I64" s="2">
-        <v>12</v>
-      </c>
-      <c r="M64" s="9"/>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D65" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="F65" s="2">
-        <v>18</v>
-      </c>
-      <c r="G65" s="2">
-        <v>18</v>
-      </c>
-      <c r="H65" s="2">
-        <v>18</v>
-      </c>
-      <c r="I65" s="2">
-        <v>18</v>
-      </c>
-      <c r="M65" s="9"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="E66" s="32"/>
-      <c r="F66" s="2">
-        <v>400</v>
-      </c>
-      <c r="G66" s="2">
-        <v>400</v>
-      </c>
-      <c r="H66" s="2">
-        <v>400</v>
-      </c>
-      <c r="I66" s="2">
-        <v>400</v>
-      </c>
-      <c r="M66" s="9"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="D67" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="E67" s="32"/>
-      <c r="F67" s="2">
-        <v>32400</v>
-      </c>
-      <c r="G67" s="2">
-        <v>32400</v>
-      </c>
-      <c r="H67" s="2">
-        <v>32400</v>
-      </c>
-      <c r="I67" s="2">
-        <v>32400</v>
-      </c>
-      <c r="M67" s="9"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="2">
-        <v>64800</v>
-      </c>
-      <c r="G68" s="2">
-        <v>64800</v>
-      </c>
-      <c r="H68" s="2">
-        <v>64800</v>
-      </c>
-      <c r="I68" s="2">
-        <v>64800</v>
-      </c>
-      <c r="M68" s="9"/>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="D69" s="32"/>
-      <c r="F69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A70" s="25"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
-      <c r="I70" s="25"/>
-      <c r="J70" s="25"/>
-      <c r="K70" s="25"/>
-      <c r="L70" s="25"/>
-      <c r="M70" s="11"/>
-    </row>
-    <row r="72" spans="1:13" ht="16.5" thickBot="1"/>
-    <row r="73" spans="1:13">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="18"/>
-      <c r="L73" s="18"/>
-      <c r="M73" s="34"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8">
-        <v>2</v>
-      </c>
-      <c r="G74" s="8">
-        <v>4</v>
-      </c>
-      <c r="H74" s="8">
-        <v>3</v>
-      </c>
-      <c r="I74" s="8">
-        <v>4</v>
-      </c>
-      <c r="J74" s="8">
-        <v>3</v>
-      </c>
-      <c r="K74" s="8">
-        <v>3</v>
-      </c>
-      <c r="L74" s="8">
-        <v>4</v>
-      </c>
-      <c r="M74" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H75" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="I75" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="J75" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K75" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="L75" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M75" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="F76" s="2">
-        <v>456</v>
-      </c>
-      <c r="G76" s="2">
-        <v>324</v>
-      </c>
-      <c r="M76" s="9"/>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E77" s="32"/>
-      <c r="F77" s="2">
-        <v>1</v>
-      </c>
-      <c r="G77" s="2">
-        <v>2</v>
-      </c>
-      <c r="M77" s="9"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="E78" s="32"/>
-      <c r="F78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M78" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="25"/>
-      <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="11"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-    </row>
-    <row r="81" spans="1:13" ht="16.5" thickBot="1">
-      <c r="D81" s="32"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="18"/>
-      <c r="L82" s="18"/>
-      <c r="M82" s="34"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="2">
-        <v>1</v>
-      </c>
-      <c r="G83" s="2">
-        <v>2</v>
-      </c>
-      <c r="M83" s="9"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="D84" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="E84" s="32"/>
-      <c r="F84" s="2">
-        <v>3000</v>
-      </c>
-      <c r="M84" s="9"/>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="D85" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="E85" s="32"/>
-      <c r="F85" s="2">
-        <v>1</v>
-      </c>
-      <c r="M85" s="9"/>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="E86" s="32"/>
-      <c r="F86" s="2">
-        <v>10000</v>
-      </c>
-      <c r="M86" s="9"/>
+      <c r="M86" s="35"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="31" t="s">
+      <c r="A87" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="E87" s="32"/>
-      <c r="F87" s="2">
+      <c r="E87" s="37"/>
+      <c r="F87" s="30">
         <v>25000</v>
       </c>
-      <c r="M87" s="9"/>
+      <c r="M87" s="35"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="31" t="s">
+      <c r="A88" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E88" s="32"/>
-      <c r="F88" s="2">
+      <c r="E88" s="37"/>
+      <c r="F88" s="30">
         <v>1500</v>
       </c>
-      <c r="M88" s="9"/>
+      <c r="M88" s="35"/>
     </row>
     <row r="89" spans="1:13">
-      <c r="E89" s="32"/>
-      <c r="F89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M89" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A90" s="25"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="26"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="25"/>
-      <c r="I90" s="25"/>
-      <c r="J90" s="25"/>
-      <c r="K90" s="25"/>
-      <c r="L90" s="25"/>
-      <c r="M90" s="11"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="H89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L89" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M89" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="17" thickBot="1">
+      <c r="A90" s="38"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
+      <c r="L90" s="38"/>
+      <c r="M90" s="42"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:J34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:J34" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Opening, Closing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:M42 F51:M51 F61:M61 F74:M74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:M42 F51:M51 F61:M61 F74:M74" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"1, 2, 3, 4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:M43 F52:M52 F62:M62 F75:M75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:M43 F52:M52 F62:M62 F75:M75" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"Inbound, Outbound"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>